<commit_message>
Updated BGR model - 2025-07-29 06:34
</commit_message>
<xml_diff>
--- a/VerveStacks_BGR/vt_vervestacks_BGR_v1.xlsx
+++ b/VerveStacks_BGR/vt_vervestacks_BGR_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_BGR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2275C336-1955-42A0-B4F0-DC2ED04CE8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A382EFFF-6804-4ED8-AD8A-8B1DDE87A5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{CF06E2E0-A394-40F6-AB79-27B4AB518F13}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{73C19F8C-0F2C-4A37-86FD-8AA5C509D0C5}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -1074,7 +1074,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54D76A79-985D-4552-A9C8-F65872EAEE2E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F799FED9-C13A-4606-AC68-AA4D8885A748}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -3999,7 +3999,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E76FE72C-1F5C-4A2D-B732-CD3840464AF5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7664A2D6-5207-487F-83B3-DB683A2E6E80}">
   <dimension ref="A2:T33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5756,7 +5756,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DAD7869-A325-475F-8955-ED84EC0793A9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63DD042-7226-4E35-9E08-81313387ACBE}">
   <dimension ref="A2:S85"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated BGR model - 2025-07-29 06:49
</commit_message>
<xml_diff>
--- a/VerveStacks_BGR/vt_vervestacks_BGR_v1.xlsx
+++ b/VerveStacks_BGR/vt_vervestacks_BGR_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_BGR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E6D5139-3A4D-4983-B6BF-770658AC3CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3FAA90E-105B-4EE5-92E3-FB4DFC128780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{34F044B6-4439-4B92-AE1B-FC0F3F3B3D1E}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{90DFCF55-610D-4375-A026-A1129868227A}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -1074,7 +1074,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6FB4C85-71D6-46DD-B94B-18C06C5C7EDA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE8081FC-BB9F-46EE-A525-E2B0D9C2A534}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -3999,7 +3999,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED6F121-FBEB-4446-A774-555D952E770C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E69E8877-E15B-4D28-B5F0-915C6E766FD0}">
   <dimension ref="A2:T33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5756,7 +5756,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE401BD5-D802-4024-A408-271FF423F41F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8391BE1D-9F63-4487-B033-557E61103735}">
   <dimension ref="A2:S85"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated BGR model - 2025-07-29 06:53
</commit_message>
<xml_diff>
--- a/VerveStacks_BGR/vt_vervestacks_BGR_v1.xlsx
+++ b/VerveStacks_BGR/vt_vervestacks_BGR_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_BGR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3FAA90E-105B-4EE5-92E3-FB4DFC128780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1077B664-4233-40D0-969D-F69CA8191BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{90DFCF55-610D-4375-A026-A1129868227A}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{39B2BE46-3996-4066-9D1F-728FF310CCDF}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -1074,7 +1074,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE8081FC-BB9F-46EE-A525-E2B0D9C2A534}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7707A553-FAAD-48EC-887E-37EAC7F2AC40}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -3999,7 +3999,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E69E8877-E15B-4D28-B5F0-915C6E766FD0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{943DFE4B-26BB-4BEF-AFAC-8347855FFBC9}">
   <dimension ref="A2:T33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5756,7 +5756,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8391BE1D-9F63-4487-B033-557E61103735}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AFCB00C-31CF-456A-9EFC-CEE765D2D106}">
   <dimension ref="A2:S85"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated BGR model - 2025-07-29 07:29
</commit_message>
<xml_diff>
--- a/VerveStacks_BGR/vt_vervestacks_BGR_v1.xlsx
+++ b/VerveStacks_BGR/vt_vervestacks_BGR_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_BGR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2BCBBBF2-5290-40CA-B5BC-2F6DAED73A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6421E881-994D-4F25-8259-29312DEE363B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{141C8834-36F3-4C16-BCCD-438BD6F701C2}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{137D42E4-F5D1-4781-9D60-3A3A28FAA422}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -1074,7 +1074,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FFC1EE6-777C-489D-A0DF-FDF915B68F48}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B97DD0D-4B73-49BE-90A0-AE15DA3811A0}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -3999,7 +3999,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2005968D-E36C-4B53-B9CF-07BA321F920F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5DDB59-107E-4005-857E-91736AC07B4B}">
   <dimension ref="A2:T33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5756,7 +5756,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6F6D8A-967F-4189-B1EB-61EB2EC64789}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E14C94-E476-4243-83B7-F8BD2B7D1A2D}">
   <dimension ref="A2:S85"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated BGR model - 2025-07-29 09:55
</commit_message>
<xml_diff>
--- a/VerveStacks_BGR/vt_vervestacks_BGR_v1.xlsx
+++ b/VerveStacks_BGR/vt_vervestacks_BGR_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_BGR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A514A837-13F4-425B-8519-D786814A1EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{90E79160-19F6-41B1-9002-80C2268146B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{90EB0C0D-373F-480B-ABAE-060D874D616A}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{D9096031-DA0D-42A9-B11D-38F4171C7619}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -1074,7 +1074,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20251CD3-A9D4-4876-ADDA-74A4998A3E4B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26EC68AD-5359-474C-BD88-BAA1C0371C43}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -3999,7 +3999,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{514334C0-C4F9-4AAE-BA1C-7F06F6A8154C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BB392C-A472-4A6D-920B-239287C188AD}">
   <dimension ref="A2:T33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5756,7 +5756,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34DC684E-4F87-4A25-9B08-6568F21B00CF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EF97E32-0F7A-474F-BDA5-855DA2D621D2}">
   <dimension ref="A2:S85"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated BGR model - 2025-07-29 14:40
</commit_message>
<xml_diff>
--- a/VerveStacks_BGR/vt_vervestacks_BGR_v1.xlsx
+++ b/VerveStacks_BGR/vt_vervestacks_BGR_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_BGR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C13F8DBB-6A8E-4F13-9EBF-C2F013183293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FEDD27D-BE0B-4EE8-8266-13EE8785B9CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{F7D45A00-6066-4510-B01C-0291BE31BC76}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{C323ABDF-0069-4E1D-BFE2-C1D7C4BA9F11}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -1074,7 +1074,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80101AC9-B77E-4C27-A0A5-F0C312E2B2E7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D3397F2-EBDD-47E5-923E-8B6D105E5EB5}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -3999,7 +3999,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A2178E-E626-4EC6-A684-D247FED6AD6E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6327E5A-1A18-41CC-AA9A-E3089069D409}">
   <dimension ref="A2:T33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5756,7 +5756,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FFE627C-C469-4B26-9545-5861D6AAE9C2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7851E1E5-81A3-4BD0-9C7C-2C1CB6BB1BC1}">
   <dimension ref="A2:S85"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated BGR model - 2025-08-03 15:14
</commit_message>
<xml_diff>
--- a/VerveStacks_BGR/vt_vervestacks_BGR_v1.xlsx
+++ b/VerveStacks_BGR/vt_vervestacks_BGR_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_BGR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2AD9F2B-C607-4DC7-B31D-DE22A09F7BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{55751A54-74F6-45DC-9534-03EAA2A78608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{8FDE7F57-12AA-472F-B157-6F620ECD01C8}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{3EA507D8-872F-4F56-B117-FF8BD6B968BF}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -696,7 +696,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0E2282-5C75-4541-895D-DC2C409A3528}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC24AD10-A5B8-4A9D-8180-0BB1C448069D}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -3621,7 +3621,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE4A72B4-AE05-4033-97B8-C8DC2137F4AD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47754E4F-9321-455D-B181-F702BFF3CB7A}">
   <dimension ref="A2:T8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3978,7 +3978,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97457CF6-C771-4B95-A870-F257979132F9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F0AEF48-58C6-4651-9AA4-DC903D2673E3}">
   <dimension ref="A2:S75"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>